<commit_message>
# Updated dev excel
</commit_message>
<xml_diff>
--- a/source/end/GeekQuiz.Office/StatisticsDev.xlsx
+++ b/source/end/GeekQuiz.Office/StatisticsDev.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\office\GeekQuiz.Office\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\r\dpe\microsoft-web\DEMO-GeekQuiz-Excel-front-end\source\end\GeekQuiz.Office\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -172,20 +172,53 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$C$1</c:f>
@@ -232,11 +265,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1396028512"/>
-        <c:axId val="1396030144"/>
+        <c:axId val="210013808"/>
+        <c:axId val="210010544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1396028512"/>
+        <c:axId val="210013808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1396030144"/>
+        <c:crossAx val="210010544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -287,7 +320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1396030144"/>
+        <c:axId val="210010544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -338,7 +371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1396028512"/>
+        <c:crossAx val="210013808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2080,9 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>